<commit_message>
Modificación menor de plantilla
</commit_message>
<xml_diff>
--- a/_estadistica-espacial/datos/CabreraTorresKennethRoy.xlsx
+++ b/_estadistica-espacial/datos/CabreraTorresKennethRoy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">nombre_var</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">potencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dist_maxima</t>
   </si>
 </sst>
 </file>
@@ -61,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,19 +146,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.0561224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,11 +189,14 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>